<commit_message>
Self-assessment sprint C + pdf MDISC
</commit_message>
<xml_diff>
--- a/docs/sprintC/PI-2023-24 Self-Assessment_SPRINT_C.xlsx
+++ b/docs/sprintC/PI-2023-24 Self-Assessment_SPRINT_C.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\IdeaProjects\lei-24-s2-1nb-g312\docs\sprintC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC46509-712E-4509-96C8-A3561144ACEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA76A6A-6DE7-4063-80E2-5821E9E8EB5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1773,8 +1773,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -1915,7 +1915,7 @@
         <v>1230932</v>
       </c>
       <c r="D10" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="38">
         <v>5</v>
@@ -1939,7 +1939,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="50">
         <f>AVERAGE(D10:R10)</f>
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="16.2" thickBot="1">
@@ -1951,7 +1951,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F11" s="35">
         <v>5</v>
@@ -1972,7 +1972,7 @@
       <c r="R11" s="10"/>
       <c r="S11" s="51">
         <f t="shared" ref="S11:S24" si="0">AVERAGE(D11:R11)</f>
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="16.2" thickBot="1">
@@ -1987,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G12" s="35">
         <v>5</v>
@@ -2005,7 +2005,7 @@
       <c r="R12" s="10"/>
       <c r="S12" s="51">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="16.2" thickBot="1">
@@ -2024,7 +2024,7 @@
         <v>5</v>
       </c>
       <c r="G13" s="36">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="35"/>
       <c r="I13" s="8"/>
@@ -2039,7 +2039,7 @@
       <c r="R13" s="10"/>
       <c r="S13" s="51">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.2" thickBot="1">
@@ -2324,19 +2324,19 @@
       </c>
       <c r="D25" s="46">
         <f>AVERAGE(D10:D24)</f>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="E25" s="46">
         <f t="shared" ref="E25:R25" si="1">AVERAGE(E10:E24)</f>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="H25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -2472,8 +2472,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6"/>
@@ -3054,8 +3054,12 @@
       <c r="A22" s="14">
         <v>17</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
+      <c r="B22" s="29">
+        <v>1201925</v>
+      </c>
+      <c r="C22" s="29">
+        <v>5</v>
+      </c>
       <c r="D22" s="59"/>
       <c r="E22" s="14" t="s">
         <v>39</v>
@@ -3080,8 +3084,12 @@
       <c r="A23" s="14">
         <v>18</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
+      <c r="B23" s="29">
+        <v>1222183</v>
+      </c>
+      <c r="C23" s="29">
+        <v>5</v>
+      </c>
       <c r="D23" s="59"/>
       <c r="E23" s="14" t="s">
         <v>39</v>
@@ -3106,8 +3114,12 @@
       <c r="A24" s="14">
         <v>19</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
+      <c r="B24" s="29">
+        <v>1230420</v>
+      </c>
+      <c r="C24" s="29">
+        <v>5</v>
+      </c>
       <c r="D24" s="59"/>
       <c r="E24" s="14" t="s">
         <v>39</v>
@@ -3165,7 +3177,9 @@
       <c r="B26" s="29">
         <v>1222183</v>
       </c>
-      <c r="C26" s="29"/>
+      <c r="C26" s="29">
+        <v>5</v>
+      </c>
       <c r="D26" s="60"/>
       <c r="E26" s="22" t="s">
         <v>39</v>
@@ -3223,7 +3237,9 @@
       <c r="B28" s="29">
         <v>1222183</v>
       </c>
-      <c r="C28" s="29"/>
+      <c r="C28" s="29">
+        <v>5</v>
+      </c>
       <c r="D28" s="60"/>
       <c r="E28" s="22" t="s">
         <v>39</v>
@@ -3251,7 +3267,9 @@
       <c r="B29" s="29">
         <v>1201925</v>
       </c>
-      <c r="C29" s="29"/>
+      <c r="C29" s="29">
+        <v>5</v>
+      </c>
       <c r="D29" s="60"/>
       <c r="E29" s="22" t="s">
         <v>39</v>
@@ -3279,7 +3297,9 @@
       <c r="B30" s="29">
         <v>1201925</v>
       </c>
-      <c r="C30" s="29"/>
+      <c r="C30" s="29">
+        <v>5</v>
+      </c>
       <c r="D30" s="60"/>
       <c r="E30" s="22" t="s">
         <v>39</v>
@@ -3307,7 +3327,9 @@
       <c r="B31" s="29">
         <v>1230420</v>
       </c>
-      <c r="C31" s="29"/>
+      <c r="C31" s="29">
+        <v>5</v>
+      </c>
       <c r="D31" s="60"/>
       <c r="E31" s="22" t="s">
         <v>39</v>
@@ -3335,7 +3357,9 @@
       <c r="B32" s="29">
         <v>1230420</v>
       </c>
-      <c r="C32" s="29"/>
+      <c r="C32" s="29">
+        <v>5</v>
+      </c>
       <c r="D32" s="60"/>
       <c r="E32" s="22" t="s">
         <v>39</v>
@@ -3363,7 +3387,9 @@
       <c r="B33" s="29">
         <v>1230420</v>
       </c>
-      <c r="C33" s="29"/>
+      <c r="C33" s="29">
+        <v>5</v>
+      </c>
       <c r="D33" s="60"/>
       <c r="E33" s="22" t="s">
         <v>39</v>
@@ -3391,7 +3417,9 @@
       <c r="B34" s="29">
         <v>1222183</v>
       </c>
-      <c r="C34" s="29"/>
+      <c r="C34" s="29">
+        <v>5</v>
+      </c>
       <c r="D34" s="60"/>
       <c r="E34" s="22" t="s">
         <v>39</v>
@@ -3450,8 +3478,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
@@ -3661,7 +3689,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E5" s="25">
         <v>5</v>
@@ -3682,7 +3710,7 @@
       <c r="Q5" s="25"/>
       <c r="R5" s="27">
         <f t="shared" si="0"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="S5" s="7" t="s">
         <v>58</v>
@@ -3713,16 +3741,16 @@
         <v>0.5</v>
       </c>
       <c r="C6" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" s="25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -3737,7 +3765,7 @@
       <c r="Q6" s="25"/>
       <c r="R6" s="27">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S6" s="7" t="s">
         <v>65</v>
@@ -3825,19 +3853,19 @@
       </c>
       <c r="C8" s="7">
         <f t="shared" ref="C8:Q8" si="1">SUMPRODUCT(C4:C7,$B$4:$B$7)</f>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="1"/>
-        <v>4.3</v>
+        <v>5</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
@@ -3900,19 +3928,19 @@
       <c r="B9" s="23"/>
       <c r="C9" s="23">
         <f>C8/5*20</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="23">
         <f t="shared" ref="D9:Q9" si="2">D8/5*20</f>
-        <v>17.2</v>
+        <v>20</v>
       </c>
       <c r="E9" s="23">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F9" s="23">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G9" s="23">
         <f t="shared" si="2"/>
@@ -4899,25 +4927,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="562c49d2-6934-4c91-8ced-1dfd11992256">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100058C7776D8E86F4DA7FFD9FA3AD9EDF2" ma:contentTypeVersion="10" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="9f79eb7164a6074f7adfeeb339facc6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="562c49d2-6934-4c91-8ced-1dfd11992256" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a9719b8ff13495842098165c74d99f4" ns2:_="">
     <xsd:import namespace="562c49d2-6934-4c91-8ced-1dfd11992256"/>
@@ -5095,10 +5104,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="562c49d2-6934-4c91-8ced-1dfd11992256">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A50E83-D78D-4190-BBA2-FA3E7056060E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="562c49d2-6934-4c91-8ced-1dfd11992256"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5120,19 +5158,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A3A50E83-D78D-4190-BBA2-FA3E7056060E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="562c49d2-6934-4c91-8ced-1dfd11992256"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>